<commit_message>
[12.12.2023][add Accepted with warning flow]
</commit_message>
<xml_diff>
--- a/ZATCA/src/test/resources/TestDataFiles/TestData.xlsx
+++ b/ZATCA/src/test/resources/TestDataFiles/TestData.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27029"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49B6528E-3931-427C-9013-8004AB1B2143}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD7BAF07-C4A3-4C91-8368-A1E4FA0910EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="41">
   <si>
     <t>RunMode</t>
   </si>
@@ -23,9 +23,6 @@
     <t>TestCaseName</t>
   </si>
   <si>
-    <t>testCSIDStandardInvoice</t>
-  </si>
-  <si>
     <t>invoiceFileName</t>
   </si>
   <si>
@@ -50,9 +47,6 @@
     <t>csr-config-example-EN.properties</t>
   </si>
   <si>
-    <t>testCSIDSimplifiedInvoice</t>
-  </si>
-  <si>
     <t>Simplified_Invoice.xml</t>
   </si>
   <si>
@@ -65,9 +59,6 @@
     <t>csr-config-example-EN-simplified.properties</t>
   </si>
   <si>
-    <t>testCSIDBothInvoice</t>
-  </si>
-  <si>
     <t>standardInvoiceFileName</t>
   </si>
   <si>
@@ -111,6 +102,42 @@
   </si>
   <si>
     <t>SIMPLIFIEDDEBIT</t>
+  </si>
+  <si>
+    <t>BR-KSA-20_Standard_Note.xml</t>
+  </si>
+  <si>
+    <t>testCSIDStandardAcceptedInvoice</t>
+  </si>
+  <si>
+    <t>testCSIDSimplifiedAcceptedInvoice</t>
+  </si>
+  <si>
+    <t>testCSIDBothAcceptedInvoice</t>
+  </si>
+  <si>
+    <t>testCSIDStandardWarningInvoice</t>
+  </si>
+  <si>
+    <t>BR-KSA-36.xml</t>
+  </si>
+  <si>
+    <t>BR-KSA-35_BR-KSA-15.xml</t>
+  </si>
+  <si>
+    <t>BR-KSA-35.xml</t>
+  </si>
+  <si>
+    <t>BR-KSA-56.xml</t>
+  </si>
+  <si>
+    <t>testCSIDSimplifiedWarningInvoice</t>
+  </si>
+  <si>
+    <t>BR-KSA-83_BR-KSA-F-06-C16.xml</t>
+  </si>
+  <si>
+    <t>testCSIDBothWarningInvoice</t>
   </si>
 </sst>
 </file>
@@ -186,14 +213,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -498,10 +524,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J15"/>
+  <dimension ref="A1:J22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -528,260 +554,424 @@
     </row>
     <row r="2" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
-        <v>2</v>
+        <v>30</v>
       </c>
       <c r="B2" s="2"/>
       <c r="C2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="E2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="2" t="s">
-        <v>5</v>
-      </c>
       <c r="F2" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
     </row>
     <row r="3" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A3" s="3" t="s">
-        <v>2</v>
+        <v>30</v>
       </c>
       <c r="B3" s="3" t="b">
         <v>1</v>
       </c>
       <c r="C3" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D3" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="D3" s="3" t="s">
+      <c r="E3" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="E3" s="3" t="s">
-        <v>8</v>
-      </c>
       <c r="F3" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G3" s="5" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
     </row>
     <row r="4" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
-        <v>11</v>
+        <v>31</v>
       </c>
       <c r="B4" s="2"/>
       <c r="C4" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D4" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D4" s="2" t="s">
+      <c r="E4" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="E4" s="2" t="s">
-        <v>5</v>
-      </c>
       <c r="F4" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
     </row>
     <row r="5" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A5" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="B5" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D5" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B5" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="C5" s="3" t="s">
+      <c r="E5" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="D5" s="3" t="s">
+      <c r="F5" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="E5" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="F5" s="3" t="s">
-        <v>15</v>
-      </c>
       <c r="G5" s="5" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
     </row>
     <row r="6" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A6" s="2" t="s">
-        <v>16</v>
+        <v>32</v>
       </c>
       <c r="B6" s="2"/>
       <c r="C6" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D6" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D6" s="2" t="s">
+      <c r="E6" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="E6" s="2" t="s">
-        <v>5</v>
-      </c>
       <c r="F6" s="2" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="G6" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="H6" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="I6" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="J6" s="2" t="s">
         <v>18</v>
-      </c>
-      <c r="H6" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="I6" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="J6" s="2" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="7" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A7" s="3" t="s">
-        <v>16</v>
+        <v>32</v>
       </c>
       <c r="B7" s="3" t="b">
         <v>1</v>
       </c>
       <c r="C7" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E7" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="D7" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="E7" s="3" t="s">
-        <v>14</v>
-      </c>
       <c r="F7" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="G7" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="G7" s="3" t="s">
+      <c r="H7" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="H7" s="3" t="s">
-        <v>8</v>
-      </c>
       <c r="I7" s="3" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="J7" s="5" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A8" s="2" t="s">
-        <v>23</v>
+        <v>33</v>
       </c>
       <c r="B8" s="2"/>
       <c r="C8" s="2" t="s">
-        <v>24</v>
+        <v>2</v>
       </c>
       <c r="D8" s="2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="E8" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="G8" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A9" s="3" t="s">
-        <v>23</v>
+        <v>33</v>
       </c>
       <c r="B9" s="3" t="b">
         <v>1</v>
       </c>
-      <c r="C9" s="6" t="s">
-        <v>25</v>
+      <c r="C9" s="3" t="s">
+        <v>35</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A10" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="B10" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="C10" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="D10" s="3" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
+        <v>34</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="F9" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="G9" s="5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A10" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="B10" s="2"/>
+      <c r="C10" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="G10" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A11" s="3" t="s">
-        <v>23</v>
+        <v>38</v>
       </c>
       <c r="B11" s="3" t="b">
         <v>1</v>
       </c>
-      <c r="C11" s="6" t="s">
-        <v>27</v>
+      <c r="C11" s="3" t="s">
+        <v>36</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.35">
+        <v>39</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="F11" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="G11" s="5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A12" s="2" t="s">
-        <v>28</v>
+        <v>40</v>
       </c>
       <c r="B12" s="2"/>
       <c r="C12" s="2" t="s">
-        <v>24</v>
+        <v>2</v>
       </c>
       <c r="D12" s="2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="E12" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F12" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G12" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="H12" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="I12" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="J12" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A13" s="3" t="s">
-        <v>28</v>
+        <v>40</v>
       </c>
       <c r="B13" s="3" t="b">
         <v>1</v>
       </c>
-      <c r="C13" s="6" t="s">
-        <v>29</v>
+      <c r="C13" s="3" t="s">
+        <v>36</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>12</v>
+        <v>39</v>
+      </c>
+      <c r="E13" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="F13" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="G13" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="H13" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="I13" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="J13" s="5" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A14" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="B14" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="C14" s="6" t="s">
-        <v>30</v>
-      </c>
-      <c r="D14" s="3" t="s">
-        <v>13</v>
+      <c r="A14" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B14" s="2"/>
+      <c r="C14" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A15" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="B15" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D15" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A16" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="B16" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="D16" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A17" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="B17" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="D17" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A18" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="B18" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D18" s="3" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A19" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B19" s="2"/>
+      <c r="C19" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A20" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="B20" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="C20" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="D20" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A21" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="B21" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="C21" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="D21" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A22" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="B22" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="C22" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="B15" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="C15" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="D15" s="3" t="s">
-        <v>14</v>
+      <c r="D22" s="3" t="s">
+        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
[13.12.2023][Add clearence & reporting for warning invoices]
</commit_message>
<xml_diff>
--- a/ZATCA/src/test/resources/TestDataFiles/TestData.xlsx
+++ b/ZATCA/src/test/resources/TestDataFiles/TestData.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27029"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD7BAF07-C4A3-4C91-8368-A1E4FA0910EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D41035FD-CA2B-4498-8980-7B1BE017E5C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="43">
   <si>
     <t>RunMode</t>
   </si>
@@ -104,9 +104,6 @@
     <t>SIMPLIFIEDDEBIT</t>
   </si>
   <si>
-    <t>BR-KSA-20_Standard_Note.xml</t>
-  </si>
-  <si>
     <t>testCSIDStandardAcceptedInvoice</t>
   </si>
   <si>
@@ -138,6 +135,15 @@
   </si>
   <si>
     <t>testCSIDBothWarningInvoice</t>
+  </si>
+  <si>
+    <t>testWarningClearanceInvoice</t>
+  </si>
+  <si>
+    <t>BR-KSA-20.xml</t>
+  </si>
+  <si>
+    <t>testWarningReportingInvoice</t>
   </si>
 </sst>
 </file>
@@ -213,13 +219,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -524,10 +531,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J22"/>
+  <dimension ref="A1:J31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -554,7 +561,7 @@
     </row>
     <row r="2" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B2" s="2"/>
       <c r="C2" s="2" t="s">
@@ -575,7 +582,7 @@
     </row>
     <row r="3" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A3" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B3" s="3" t="b">
         <v>1</v>
@@ -598,7 +605,7 @@
     </row>
     <row r="4" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B4" s="2"/>
       <c r="C4" s="2" t="s">
@@ -619,7 +626,7 @@
     </row>
     <row r="5" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A5" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B5" s="3" t="b">
         <v>1</v>
@@ -642,7 +649,7 @@
     </row>
     <row r="6" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A6" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B6" s="2"/>
       <c r="C6" s="2" t="s">
@@ -672,7 +679,7 @@
     </row>
     <row r="7" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A7" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B7" s="3" t="b">
         <v>1</v>
@@ -704,7 +711,7 @@
     </row>
     <row r="8" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A8" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B8" s="2"/>
       <c r="C8" s="2" t="s">
@@ -725,19 +732,19 @@
     </row>
     <row r="9" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A9" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="B9" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="D9" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="B9" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="C9" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="D9" s="3" t="s">
-        <v>34</v>
-      </c>
       <c r="E9" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F9" s="3" t="s">
         <v>9</v>
@@ -748,7 +755,7 @@
     </row>
     <row r="10" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A10" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B10" s="2"/>
       <c r="C10" s="2" t="s">
@@ -769,19 +776,19 @@
     </row>
     <row r="11" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A11" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="B11" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="D11" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="B11" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="C11" s="3" t="s">
+      <c r="E11" s="3" t="s">
         <v>36</v>
-      </c>
-      <c r="D11" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="E11" s="3" t="s">
-        <v>37</v>
       </c>
       <c r="F11" s="3" t="s">
         <v>13</v>
@@ -792,7 +799,7 @@
     </row>
     <row r="12" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A12" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B12" s="2"/>
       <c r="C12" s="2" t="s">
@@ -822,28 +829,28 @@
     </row>
     <row r="13" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A13" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B13" s="3" t="b">
         <v>1</v>
       </c>
       <c r="C13" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="E13" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="D13" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="E13" s="3" t="s">
-        <v>37</v>
-      </c>
       <c r="F13" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="G13" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="H13" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="I13" s="3" t="s">
         <v>17</v>
@@ -907,29 +914,29 @@
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A18" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="B18" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="C18" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="D18" s="3" t="s">
-        <v>29</v>
+      <c r="A18" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B18" s="2"/>
+      <c r="C18" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A19" s="2" t="s">
+      <c r="A19" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="B19" s="2"/>
-      <c r="C19" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="D19" s="2" t="s">
-        <v>2</v>
+      <c r="B19" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="C19" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="D19" s="3" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.35">
@@ -940,10 +947,10 @@
         <v>1</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.35">
@@ -954,24 +961,146 @@
         <v>1</v>
       </c>
       <c r="C21" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="D21" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A22" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="B22" s="2"/>
+      <c r="C22" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D22" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A23" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="B23" s="6" t="b">
+        <v>1</v>
+      </c>
+      <c r="C23" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D23" s="3" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A24" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="B24" s="6" t="b">
+        <v>1</v>
+      </c>
+      <c r="C24" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D24" s="3" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A25" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="B25" s="6" t="b">
+        <v>1</v>
+      </c>
+      <c r="C25" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D25" s="3" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A26" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="B26" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="C26" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="D26" s="3" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A27" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="B27" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="C27" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="D27" s="3" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A28" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="B28" s="2"/>
+      <c r="C28" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D28" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A29" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="B29" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="C29" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="D29" s="3" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A30" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="B30" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="C30" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="D21" s="3" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A22" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="B22" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="C22" s="3" t="s">
+      <c r="D30" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A31" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="B31" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="C31" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="D22" s="3" t="s">
-        <v>12</v>
+      <c r="D31" s="3" t="s">
+        <v>36</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
[22.1.2024][Add Error invoice Scenarios]
</commit_message>
<xml_diff>
--- a/ZATCA/src/test/resources/TestDataFiles/TestData.xlsx
+++ b/ZATCA/src/test/resources/TestDataFiles/TestData.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27126"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D41035FD-CA2B-4498-8980-7B1BE017E5C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B7E7EA8-4CBB-4F5D-8EA9-0466D4502DA3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="51">
   <si>
     <t>RunMode</t>
   </si>
@@ -144,6 +144,30 @@
   </si>
   <si>
     <t>testWarningReportingInvoice</t>
+  </si>
+  <si>
+    <t>testErrorClearanceInvoice</t>
+  </si>
+  <si>
+    <t>testErrorReportingInvoice</t>
+  </si>
+  <si>
+    <t>BR-KSA-F-06-C17.xml</t>
+  </si>
+  <si>
+    <t>BR-KSA-EN16931-08.xml</t>
+  </si>
+  <si>
+    <t>BR-CL-03.xml</t>
+  </si>
+  <si>
+    <t>BR-KSA-49.xml</t>
+  </si>
+  <si>
+    <t>BR-KSA-72.xml</t>
+  </si>
+  <si>
+    <t>BR-KSA-06.xml</t>
   </si>
 </sst>
 </file>
@@ -219,14 +243,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -531,10 +554,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J31"/>
+  <dimension ref="A1:J39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="B25" sqref="B25"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="B40" sqref="B40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -983,7 +1006,7 @@
       <c r="A23" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="B23" s="6" t="b">
+      <c r="B23" s="3" t="b">
         <v>1</v>
       </c>
       <c r="C23" s="3" t="s">
@@ -997,7 +1020,7 @@
       <c r="A24" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="B24" s="6" t="b">
+      <c r="B24" s="3" t="b">
         <v>1</v>
       </c>
       <c r="C24" s="3" t="s">
@@ -1011,7 +1034,7 @@
       <c r="A25" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="B25" s="6" t="b">
+      <c r="B25" s="3" t="b">
         <v>1</v>
       </c>
       <c r="C25" s="3" t="s">
@@ -1101,6 +1124,114 @@
       </c>
       <c r="D31" s="3" t="s">
         <v>36</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A32" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="B32" s="2"/>
+      <c r="C32" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D32" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A33" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="B33" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="C33" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D33" s="3" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A34" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="B34" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="C34" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="D34" s="3" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A35" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="B35" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="C35" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="D35" s="3" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A36" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="B36" s="2"/>
+      <c r="C36" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D36" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A37" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="B37" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="C37" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="D37" s="3" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A38" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="B38" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="C38" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="D38" s="3" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A39" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="B39" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="C39" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="D39" s="3" t="s">
+        <v>50</v>
       </c>
     </row>
   </sheetData>

</xml_diff>